<commit_message>
Timer0 & Timer2 Modules
The Service  Debounce_Handler is tested.

The Service Update_Temp Periodic Performance. is Tested .
</commit_message>
<xml_diff>
--- a/Doc/Modules Description.xlsx
+++ b/Doc/Modules Description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\GIT_Lab\Temp_Controlled_Tank\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C942C8A-43A4-4C5B-A9F9-47CA3A61C3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14435731-843E-4DE9-A99A-10B8F5BD7489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D1416E92-1A25-439F-ACC6-6770CF9B0430}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1416E92-1A25-439F-ACC6-6770CF9B0430}"/>
   </bookViews>
   <sheets>
     <sheet name="EEPROM_Module" sheetId="4" r:id="rId1"/>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7D3C0C-648E-4B46-A73F-450AA85BD547}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3A04B5-4EE1-45A0-9E68-3BE512820D0D}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>